<commit_message>
fix: update timestamp. feat: add warning & unduh skl
</commit_message>
<xml_diff>
--- a/cache/data_siswa.xlsx
+++ b/cache/data_siswa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\App-Development\ceklulus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\App-Development\ceklulus\cache\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912CA5A0-B417-430F-9732-7DE3E89292CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD375E-7534-46A5-86D8-F14427D7454B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{12D39D77-401A-4D23-BD2A-539CB254051B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>nisn</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>file_pdf</t>
+  </si>
+  <si>
+    <t>status_skl</t>
+  </si>
+  <si>
+    <t>12345.pdf</t>
+  </si>
+  <si>
+    <t>12346.pdf</t>
+  </si>
+  <si>
+    <t>DITAHAN</t>
+  </si>
+  <si>
+    <t>Lorem</t>
+  </si>
+  <si>
+    <t>12347.pdf</t>
   </si>
 </sst>
 </file>
@@ -83,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,22 +109,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,73 +462,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC97B2A-D0EC-49CF-A1F8-0D61CBB6B1E8}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>12345</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
-        <v>39764</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="6">
+        <v>45779</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="str">
-        <f>A2&amp;".pdf"</f>
-        <v>12345.pdf</v>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>12346</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
-        <v>39398</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="6">
+        <v>45779</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="str">
-        <f>A3&amp;".pdf"</f>
-        <v>12346.pdf</v>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>12347</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45779</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>